<commit_message>
Made some changes in Main class and added some scenrios and made changes in Book1
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\eclipse-workspace\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5928" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,46 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
-  <si>
-    <t>USERID</t>
-  </si>
-  <si>
-    <t>EMAIL</t>
-  </si>
-  <si>
-    <t>PASSWORD</t>
-  </si>
-  <si>
-    <t>Michael@gmail.com</t>
-  </si>
-  <si>
-    <t>Anya@gmail.com</t>
-  </si>
-  <si>
-    <t>Jorge.j@gmail.com</t>
-  </si>
-  <si>
-    <t>Anna@gmail.com</t>
-  </si>
-  <si>
-    <t>helen@gmail.com</t>
-  </si>
-  <si>
-    <t>Abcde1234</t>
-  </si>
-  <si>
-    <t>Qwerty1234</t>
-  </si>
-  <si>
-    <t>Asdfg1234</t>
-  </si>
-  <si>
-    <t>Voice.123</t>
-  </si>
-  <si>
-    <t>Html1234.</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="31">
   <si>
     <t>First_Name</t>
   </si>
@@ -139,13 +101,31 @@
   </si>
   <si>
     <t>emma.wwhite@email.com</t>
+  </si>
+  <si>
+    <t>Watson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jon.smith@email.com </t>
+  </si>
+  <si>
+    <t>janee.doe@email.com</t>
+  </si>
+  <si>
+    <t>alicee.brown@email.com</t>
+  </si>
+  <si>
+    <t>bob.johnson@email.com</t>
+  </si>
+  <si>
+    <t>emma.watson@email.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -157,14 +137,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -214,23 +186,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -511,8 +477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -524,106 +490,106 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="5" t="s">
+      <c r="E5" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="4"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>30</v>
+      <c r="E6" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -633,93 +599,226 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="3" max="3" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
-        <v>12</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
+      <c r="E4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
+      <c r="C5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
-        <v>15</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>12</v>
+      <c r="E5" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="B5" r:id="rId4"/>
-    <hyperlink ref="B6" r:id="rId5"/>
+    <hyperlink ref="B2" r:id="rId1" display="Michael@gmail.com"/>
+    <hyperlink ref="B5" r:id="rId2" display="Jorge.j@gmail.com"/>
+    <hyperlink ref="B6" r:id="rId3" display="helen@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>